<commit_message>
Framework part has been completed
</commit_message>
<xml_diff>
--- a/src/main/java/com/jala/qa/testData/LoginData.xlsx
+++ b/src/main/java/com/jala/qa/testData/LoginData.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OM SAI AM\eclipse-workspace\Jala_HybridFramwork_Sept2024_Batch_7PM\src\main\java\com\jala\qa\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="3276" activeTab="2"/>
   </bookViews>
@@ -12,7 +17,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>0,0</t>
   </si>
@@ -545,7 +549,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -557,7 +561,7 @@
     <col min="2" max="2" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -565,7 +569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -573,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -581,7 +585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -589,13 +593,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>